<commit_message>
redesigned schedule part, worked on partial get_best_elective function
</commit_message>
<xml_diff>
--- a/files/District-Schedule-Template.xlsx
+++ b/files/District-Schedule-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boyuanliu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0526321D-210C-8043-AEB9-A51DF0E0B563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CBC2D3-17A6-1D4B-90B4-0A3A3EF394DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="4920" windowWidth="25440" windowHeight="14600" xr2:uid="{415E5FFC-11DE-134A-93DE-0D4E4D9BAD8C}"/>
+    <workbookView xWindow="2480" yWindow="460" windowWidth="25440" windowHeight="7360" xr2:uid="{415E5FFC-11DE-134A-93DE-0D4E4D9BAD8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Option 6</t>
   </si>
   <si>
-    <t>studentid</t>
-  </si>
-  <si>
     <t>art</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>ecr</t>
+  </si>
+  <si>
+    <t>bl6</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,25 +457,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>